<commit_message>
update telecom org slicing 14f1197c3e1fe609d2c7d15211db850436923e6a
</commit_message>
<xml_diff>
--- a/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-organization.xlsx
+++ b/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-organization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11037" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11037" uniqueCount="941">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-11T14:18:11+00:00</t>
+    <t>2024-10-11T14:28:17+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2245,10 +2245,6 @@
   </si>
   <si>
     <t>Human contact for the organization.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">profile:$this.resolve()}
-</t>
   </si>
   <si>
     <t>cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}
@@ -28731,7 +28727,7 @@
         <v>79</v>
       </c>
       <c r="AB212" t="s" s="2">
-        <v>718</v>
+        <v>558</v>
       </c>
       <c r="AC212" s="2"/>
       <c r="AD212" t="s" s="2">
@@ -28753,22 +28749,22 @@
         <v>212</v>
       </c>
       <c r="AJ212" t="s" s="2">
+        <v>718</v>
+      </c>
+      <c r="AK212" t="s" s="2">
         <v>719</v>
       </c>
-      <c r="AK212" t="s" s="2">
+      <c r="AL212" t="s" s="2">
         <v>720</v>
       </c>
-      <c r="AL212" t="s" s="2">
+      <c r="AM212" t="s" s="2">
         <v>721</v>
       </c>
-      <c r="AM212" t="s" s="2">
+      <c r="AN212" t="s" s="2">
         <v>722</v>
       </c>
-      <c r="AN212" t="s" s="2">
+      <c r="AO212" t="s" s="2">
         <v>723</v>
-      </c>
-      <c r="AO212" t="s" s="2">
-        <v>724</v>
       </c>
       <c r="AP212" t="s" s="2">
         <v>79</v>
@@ -28776,10 +28772,10 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B213" t="s" s="2">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" t="s" s="2">
@@ -28894,10 +28890,10 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B214" t="s" s="2">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" t="s" s="2">
@@ -29014,13 +29010,13 @@
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
+        <v>726</v>
+      </c>
+      <c r="B215" t="s" s="2">
+        <v>725</v>
+      </c>
+      <c r="C215" t="s" s="2">
         <v>727</v>
-      </c>
-      <c r="B215" t="s" s="2">
-        <v>726</v>
-      </c>
-      <c r="C215" t="s" s="2">
-        <v>728</v>
       </c>
       <c r="D215" t="s" s="2">
         <v>79</v>
@@ -29042,13 +29038,13 @@
         <v>79</v>
       </c>
       <c r="K215" t="s" s="2">
+        <v>728</v>
+      </c>
+      <c r="L215" t="s" s="2">
         <v>729</v>
       </c>
-      <c r="L215" t="s" s="2">
+      <c r="M215" t="s" s="2">
         <v>730</v>
-      </c>
-      <c r="M215" t="s" s="2">
-        <v>731</v>
       </c>
       <c r="N215" s="2"/>
       <c r="O215" s="2"/>
@@ -29134,10 +29130,10 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B216" t="s" s="2">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" t="s" s="2">
@@ -29163,10 +29159,10 @@
         <v>180</v>
       </c>
       <c r="L216" t="s" s="2">
+        <v>732</v>
+      </c>
+      <c r="M216" t="s" s="2">
         <v>733</v>
-      </c>
-      <c r="M216" t="s" s="2">
-        <v>734</v>
       </c>
       <c r="N216" s="2"/>
       <c r="O216" s="2"/>
@@ -29196,37 +29192,37 @@
         <v>325</v>
       </c>
       <c r="Y216" t="s" s="2">
+        <v>734</v>
+      </c>
+      <c r="Z216" t="s" s="2">
         <v>735</v>
       </c>
-      <c r="Z216" t="s" s="2">
+      <c r="AA216" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB216" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC216" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD216" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE216" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF216" t="s" s="2">
         <v>736</v>
       </c>
-      <c r="AA216" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AB216" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AC216" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AD216" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AE216" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF216" t="s" s="2">
+      <c r="AG216" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH216" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI216" t="s" s="2">
         <v>737</v>
-      </c>
-      <c r="AG216" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH216" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AI216" t="s" s="2">
-        <v>738</v>
       </c>
       <c r="AJ216" t="s" s="2">
         <v>103</v>
@@ -29238,13 +29234,13 @@
         <v>79</v>
       </c>
       <c r="AM216" t="s" s="2">
+        <v>738</v>
+      </c>
+      <c r="AN216" t="s" s="2">
         <v>739</v>
       </c>
-      <c r="AN216" t="s" s="2">
+      <c r="AO216" t="s" s="2">
         <v>740</v>
-      </c>
-      <c r="AO216" t="s" s="2">
-        <v>741</v>
       </c>
       <c r="AP216" t="s" s="2">
         <v>79</v>
@@ -29252,10 +29248,10 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B217" t="s" s="2">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" t="s" s="2">
@@ -29281,16 +29277,16 @@
         <v>105</v>
       </c>
       <c r="L217" t="s" s="2">
+        <v>742</v>
+      </c>
+      <c r="M217" t="s" s="2">
         <v>743</v>
       </c>
-      <c r="M217" t="s" s="2">
+      <c r="N217" t="s" s="2">
         <v>744</v>
       </c>
-      <c r="N217" t="s" s="2">
+      <c r="O217" t="s" s="2">
         <v>745</v>
-      </c>
-      <c r="O217" t="s" s="2">
-        <v>746</v>
       </c>
       <c r="P217" t="s" s="2">
         <v>79</v>
@@ -29339,7 +29335,7 @@
         <v>79</v>
       </c>
       <c r="AF217" t="s" s="2">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AG217" t="s" s="2">
         <v>80</v>
@@ -29360,10 +29356,10 @@
         <v>79</v>
       </c>
       <c r="AM217" t="s" s="2">
+        <v>747</v>
+      </c>
+      <c r="AN217" t="s" s="2">
         <v>748</v>
-      </c>
-      <c r="AN217" t="s" s="2">
-        <v>749</v>
       </c>
       <c r="AO217" t="s" s="2">
         <v>358</v>
@@ -29374,10 +29370,10 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B218" t="s" s="2">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" t="s" s="2">
@@ -29403,16 +29399,16 @@
         <v>180</v>
       </c>
       <c r="L218" t="s" s="2">
+        <v>750</v>
+      </c>
+      <c r="M218" t="s" s="2">
         <v>751</v>
       </c>
-      <c r="M218" t="s" s="2">
+      <c r="N218" t="s" s="2">
         <v>752</v>
       </c>
-      <c r="N218" t="s" s="2">
+      <c r="O218" t="s" s="2">
         <v>753</v>
-      </c>
-      <c r="O218" t="s" s="2">
-        <v>754</v>
       </c>
       <c r="P218" t="s" s="2">
         <v>79</v>
@@ -29440,28 +29436,28 @@
         <v>325</v>
       </c>
       <c r="Y218" t="s" s="2">
+        <v>754</v>
+      </c>
+      <c r="Z218" t="s" s="2">
         <v>755</v>
       </c>
-      <c r="Z218" t="s" s="2">
+      <c r="AA218" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB218" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC218" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD218" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE218" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF218" t="s" s="2">
         <v>756</v>
-      </c>
-      <c r="AA218" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AB218" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AC218" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AD218" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AE218" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF218" t="s" s="2">
-        <v>757</v>
       </c>
       <c r="AG218" t="s" s="2">
         <v>80</v>
@@ -29482,13 +29478,13 @@
         <v>79</v>
       </c>
       <c r="AM218" t="s" s="2">
+        <v>757</v>
+      </c>
+      <c r="AN218" t="s" s="2">
         <v>758</v>
       </c>
-      <c r="AN218" t="s" s="2">
+      <c r="AO218" t="s" s="2">
         <v>759</v>
-      </c>
-      <c r="AO218" t="s" s="2">
-        <v>760</v>
       </c>
       <c r="AP218" t="s" s="2">
         <v>79</v>
@@ -29496,10 +29492,10 @@
     </row>
     <row r="219" hidden="true">
       <c r="A219" t="s" s="2">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B219" t="s" s="2">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" t="s" s="2">
@@ -29522,16 +29518,16 @@
         <v>92</v>
       </c>
       <c r="K219" t="s" s="2">
+        <v>761</v>
+      </c>
+      <c r="L219" t="s" s="2">
         <v>762</v>
       </c>
-      <c r="L219" t="s" s="2">
+      <c r="M219" t="s" s="2">
         <v>763</v>
       </c>
-      <c r="M219" t="s" s="2">
+      <c r="N219" t="s" s="2">
         <v>764</v>
-      </c>
-      <c r="N219" t="s" s="2">
-        <v>765</v>
       </c>
       <c r="O219" s="2"/>
       <c r="P219" t="s" s="2">
@@ -29581,7 +29577,7 @@
         <v>79</v>
       </c>
       <c r="AF219" t="s" s="2">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AG219" t="s" s="2">
         <v>80</v>
@@ -29616,10 +29612,10 @@
     </row>
     <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B220" t="s" s="2">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" t="s" s="2">
@@ -29645,10 +29641,10 @@
         <v>234</v>
       </c>
       <c r="L220" t="s" s="2">
+        <v>767</v>
+      </c>
+      <c r="M220" t="s" s="2">
         <v>768</v>
-      </c>
-      <c r="M220" t="s" s="2">
-        <v>769</v>
       </c>
       <c r="N220" s="2"/>
       <c r="O220" s="2"/>
@@ -29699,7 +29695,7 @@
         <v>79</v>
       </c>
       <c r="AF220" t="s" s="2">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AG220" t="s" s="2">
         <v>80</v>
@@ -29723,7 +29719,7 @@
         <v>203</v>
       </c>
       <c r="AN220" t="s" s="2">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="AO220" t="s" s="2">
         <v>365</v>
@@ -29734,13 +29730,13 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B221" t="s" s="2">
         <v>712</v>
       </c>
       <c r="C221" t="s" s="2">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D221" t="s" s="2">
         <v>79</v>
@@ -29762,10 +29758,10 @@
         <v>79</v>
       </c>
       <c r="K221" t="s" s="2">
+        <v>773</v>
+      </c>
+      <c r="L221" t="s" s="2">
         <v>774</v>
-      </c>
-      <c r="L221" t="s" s="2">
-        <v>775</v>
       </c>
       <c r="M221" t="s" s="2">
         <v>715</v>
@@ -29835,7 +29831,7 @@
         <v>212</v>
       </c>
       <c r="AJ221" t="s" s="2">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="AK221" t="s" s="2">
         <v>79</v>
@@ -29844,13 +29840,13 @@
         <v>79</v>
       </c>
       <c r="AM221" t="s" s="2">
+        <v>721</v>
+      </c>
+      <c r="AN221" t="s" s="2">
         <v>722</v>
       </c>
-      <c r="AN221" t="s" s="2">
+      <c r="AO221" t="s" s="2">
         <v>723</v>
-      </c>
-      <c r="AO221" t="s" s="2">
-        <v>724</v>
       </c>
       <c r="AP221" t="s" s="2">
         <v>79</v>
@@ -29858,10 +29854,10 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B222" t="s" s="2">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" t="s" s="2">
@@ -29976,10 +29972,10 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B223" t="s" s="2">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" t="s" s="2">
@@ -30096,13 +30092,13 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B224" t="s" s="2">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C224" t="s" s="2">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D224" t="s" s="2">
         <v>79</v>
@@ -30124,13 +30120,13 @@
         <v>79</v>
       </c>
       <c r="K224" t="s" s="2">
+        <v>728</v>
+      </c>
+      <c r="L224" t="s" s="2">
         <v>729</v>
       </c>
-      <c r="L224" t="s" s="2">
+      <c r="M224" t="s" s="2">
         <v>730</v>
-      </c>
-      <c r="M224" t="s" s="2">
-        <v>731</v>
       </c>
       <c r="N224" s="2"/>
       <c r="O224" s="2"/>
@@ -30216,10 +30212,10 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
+        <v>778</v>
+      </c>
+      <c r="B225" t="s" s="2">
         <v>779</v>
-      </c>
-      <c r="B225" t="s" s="2">
-        <v>780</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" t="s" s="2">
@@ -30334,10 +30330,10 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
+        <v>780</v>
+      </c>
+      <c r="B226" t="s" s="2">
         <v>781</v>
-      </c>
-      <c r="B226" t="s" s="2">
-        <v>782</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" t="s" s="2">
@@ -30452,10 +30448,10 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
+        <v>782</v>
+      </c>
+      <c r="B227" t="s" s="2">
         <v>783</v>
-      </c>
-      <c r="B227" t="s" s="2">
-        <v>784</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" t="s" s="2">
@@ -30495,7 +30491,7 @@
       </c>
       <c r="Q227" s="2"/>
       <c r="R227" t="s" s="2">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="S227" t="s" s="2">
         <v>79</v>
@@ -30572,10 +30568,10 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
+        <v>785</v>
+      </c>
+      <c r="B228" t="s" s="2">
         <v>786</v>
-      </c>
-      <c r="B228" t="s" s="2">
-        <v>787</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" t="s" s="2">
@@ -30616,7 +30612,7 @@
         <v>79</v>
       </c>
       <c r="S228" t="s" s="2">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="T228" t="s" s="2">
         <v>79</v>
@@ -30635,7 +30631,7 @@
       </c>
       <c r="Y228" s="2"/>
       <c r="Z228" t="s" s="2">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="AA228" t="s" s="2">
         <v>79</v>
@@ -30688,13 +30684,13 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
+        <v>789</v>
+      </c>
+      <c r="B229" t="s" s="2">
+        <v>725</v>
+      </c>
+      <c r="C229" t="s" s="2">
         <v>790</v>
-      </c>
-      <c r="B229" t="s" s="2">
-        <v>726</v>
-      </c>
-      <c r="C229" t="s" s="2">
-        <v>791</v>
       </c>
       <c r="D229" t="s" s="2">
         <v>79</v>
@@ -30716,13 +30712,13 @@
         <v>79</v>
       </c>
       <c r="K229" t="s" s="2">
+        <v>791</v>
+      </c>
+      <c r="L229" t="s" s="2">
         <v>792</v>
       </c>
-      <c r="L229" t="s" s="2">
+      <c r="M229" t="s" s="2">
         <v>793</v>
-      </c>
-      <c r="M229" t="s" s="2">
-        <v>794</v>
       </c>
       <c r="N229" s="2"/>
       <c r="O229" s="2"/>
@@ -30808,10 +30804,10 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B230" t="s" s="2">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" t="s" s="2">
@@ -30926,10 +30922,10 @@
     </row>
     <row r="231" hidden="true">
       <c r="A231" t="s" s="2">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B231" t="s" s="2">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" t="s" s="2">
@@ -31046,13 +31042,13 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
+        <v>796</v>
+      </c>
+      <c r="B232" t="s" s="2">
+        <v>781</v>
+      </c>
+      <c r="C232" t="s" s="2">
         <v>797</v>
-      </c>
-      <c r="B232" t="s" s="2">
-        <v>782</v>
-      </c>
-      <c r="C232" t="s" s="2">
-        <v>798</v>
       </c>
       <c r="D232" t="s" s="2">
         <v>79</v>
@@ -31077,7 +31073,7 @@
         <v>112</v>
       </c>
       <c r="L232" t="s" s="2">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="M232" t="s" s="2">
         <v>206</v>
@@ -31166,10 +31162,10 @@
     </row>
     <row r="233" hidden="true">
       <c r="A233" t="s" s="2">
+        <v>799</v>
+      </c>
+      <c r="B233" t="s" s="2">
         <v>800</v>
-      </c>
-      <c r="B233" t="s" s="2">
-        <v>801</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" t="s" s="2">
@@ -31284,10 +31280,10 @@
     </row>
     <row r="234" hidden="true">
       <c r="A234" t="s" s="2">
+        <v>801</v>
+      </c>
+      <c r="B234" t="s" s="2">
         <v>802</v>
-      </c>
-      <c r="B234" t="s" s="2">
-        <v>803</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" t="s" s="2">
@@ -31402,10 +31398,10 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
+        <v>803</v>
+      </c>
+      <c r="B235" t="s" s="2">
         <v>804</v>
-      </c>
-      <c r="B235" t="s" s="2">
-        <v>805</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" t="s" s="2">
@@ -31445,7 +31441,7 @@
       </c>
       <c r="Q235" s="2"/>
       <c r="R235" t="s" s="2">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="S235" t="s" s="2">
         <v>79</v>
@@ -31522,10 +31518,10 @@
     </row>
     <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
+        <v>805</v>
+      </c>
+      <c r="B236" t="s" s="2">
         <v>806</v>
-      </c>
-      <c r="B236" t="s" s="2">
-        <v>807</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" t="s" s="2">
@@ -31585,7 +31581,7 @@
       </c>
       <c r="Y236" s="2"/>
       <c r="Z236" t="s" s="2">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="AA236" t="s" s="2">
         <v>79</v>
@@ -31638,10 +31634,10 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B237" t="s" s="2">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C237" t="s" s="2">
         <v>214</v>
@@ -31669,7 +31665,7 @@
         <v>112</v>
       </c>
       <c r="L237" t="s" s="2">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="M237" t="s" s="2">
         <v>206</v>
@@ -31758,10 +31754,10 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B238" t="s" s="2">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" t="s" s="2">
@@ -31876,10 +31872,10 @@
     </row>
     <row r="239" hidden="true">
       <c r="A239" t="s" s="2">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B239" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" t="s" s="2">
@@ -31994,10 +31990,10 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B240" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" t="s" s="2">
@@ -32114,10 +32110,10 @@
     </row>
     <row r="241" hidden="true">
       <c r="A241" t="s" s="2">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B241" t="s" s="2">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C241" s="2"/>
       <c r="D241" t="s" s="2">
@@ -32232,13 +32228,13 @@
     </row>
     <row r="242" hidden="true">
       <c r="A242" t="s" s="2">
+        <v>814</v>
+      </c>
+      <c r="B242" t="s" s="2">
+        <v>781</v>
+      </c>
+      <c r="C242" t="s" s="2">
         <v>815</v>
-      </c>
-      <c r="B242" t="s" s="2">
-        <v>782</v>
-      </c>
-      <c r="C242" t="s" s="2">
-        <v>816</v>
       </c>
       <c r="D242" t="s" s="2">
         <v>79</v>
@@ -32352,10 +32348,10 @@
     </row>
     <row r="243" hidden="true">
       <c r="A243" t="s" s="2">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B243" t="s" s="2">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" t="s" s="2">
@@ -32470,10 +32466,10 @@
     </row>
     <row r="244" hidden="true">
       <c r="A244" t="s" s="2">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B244" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" t="s" s="2">
@@ -32588,10 +32584,10 @@
     </row>
     <row r="245" hidden="true">
       <c r="A245" t="s" s="2">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B245" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" t="s" s="2">
@@ -32631,7 +32627,7 @@
       </c>
       <c r="Q245" s="2"/>
       <c r="R245" t="s" s="2">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="S245" t="s" s="2">
         <v>79</v>
@@ -32708,10 +32704,10 @@
     </row>
     <row r="246" hidden="true">
       <c r="A246" t="s" s="2">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B246" t="s" s="2">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" t="s" s="2">
@@ -32826,13 +32822,13 @@
     </row>
     <row r="247" hidden="true">
       <c r="A247" t="s" s="2">
+        <v>820</v>
+      </c>
+      <c r="B247" t="s" s="2">
+        <v>781</v>
+      </c>
+      <c r="C247" t="s" s="2">
         <v>821</v>
-      </c>
-      <c r="B247" t="s" s="2">
-        <v>782</v>
-      </c>
-      <c r="C247" t="s" s="2">
-        <v>822</v>
       </c>
       <c r="D247" t="s" s="2">
         <v>79</v>
@@ -32857,7 +32853,7 @@
         <v>112</v>
       </c>
       <c r="L247" t="s" s="2">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="M247" t="s" s="2">
         <v>206</v>
@@ -32946,10 +32942,10 @@
     </row>
     <row r="248" hidden="true">
       <c r="A248" t="s" s="2">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B248" t="s" s="2">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" t="s" s="2">
@@ -33064,10 +33060,10 @@
     </row>
     <row r="249" hidden="true">
       <c r="A249" t="s" s="2">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B249" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" t="s" s="2">
@@ -33182,10 +33178,10 @@
     </row>
     <row r="250" hidden="true">
       <c r="A250" t="s" s="2">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B250" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" t="s" s="2">
@@ -33225,7 +33221,7 @@
       </c>
       <c r="Q250" s="2"/>
       <c r="R250" t="s" s="2">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="S250" t="s" s="2">
         <v>79</v>
@@ -33302,10 +33298,10 @@
     </row>
     <row r="251" hidden="true">
       <c r="A251" t="s" s="2">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B251" t="s" s="2">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" t="s" s="2">
@@ -33420,13 +33416,13 @@
     </row>
     <row r="252" hidden="true">
       <c r="A252" t="s" s="2">
+        <v>827</v>
+      </c>
+      <c r="B252" t="s" s="2">
+        <v>781</v>
+      </c>
+      <c r="C252" t="s" s="2">
         <v>828</v>
-      </c>
-      <c r="B252" t="s" s="2">
-        <v>782</v>
-      </c>
-      <c r="C252" t="s" s="2">
-        <v>829</v>
       </c>
       <c r="D252" t="s" s="2">
         <v>79</v>
@@ -33540,10 +33536,10 @@
     </row>
     <row r="253" hidden="true">
       <c r="A253" t="s" s="2">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B253" t="s" s="2">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" t="s" s="2">
@@ -33658,10 +33654,10 @@
     </row>
     <row r="254" hidden="true">
       <c r="A254" t="s" s="2">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B254" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" t="s" s="2">
@@ -33776,10 +33772,10 @@
     </row>
     <row r="255" hidden="true">
       <c r="A255" t="s" s="2">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B255" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" t="s" s="2">
@@ -33819,7 +33815,7 @@
       </c>
       <c r="Q255" s="2"/>
       <c r="R255" t="s" s="2">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="S255" t="s" s="2">
         <v>79</v>
@@ -33896,10 +33892,10 @@
     </row>
     <row r="256" hidden="true">
       <c r="A256" t="s" s="2">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B256" t="s" s="2">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" t="s" s="2">
@@ -34014,13 +34010,13 @@
     </row>
     <row r="257" hidden="true">
       <c r="A257" t="s" s="2">
+        <v>833</v>
+      </c>
+      <c r="B257" t="s" s="2">
+        <v>781</v>
+      </c>
+      <c r="C257" t="s" s="2">
         <v>834</v>
-      </c>
-      <c r="B257" t="s" s="2">
-        <v>782</v>
-      </c>
-      <c r="C257" t="s" s="2">
-        <v>835</v>
       </c>
       <c r="D257" t="s" s="2">
         <v>79</v>
@@ -34045,7 +34041,7 @@
         <v>112</v>
       </c>
       <c r="L257" t="s" s="2">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="M257" t="s" s="2">
         <v>206</v>
@@ -34134,10 +34130,10 @@
     </row>
     <row r="258" hidden="true">
       <c r="A258" t="s" s="2">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B258" t="s" s="2">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" t="s" s="2">
@@ -34252,10 +34248,10 @@
     </row>
     <row r="259" hidden="true">
       <c r="A259" t="s" s="2">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B259" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" t="s" s="2">
@@ -34370,10 +34366,10 @@
     </row>
     <row r="260" hidden="true">
       <c r="A260" t="s" s="2">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B260" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" t="s" s="2">
@@ -34413,7 +34409,7 @@
       </c>
       <c r="Q260" s="2"/>
       <c r="R260" t="s" s="2">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="S260" t="s" s="2">
         <v>79</v>
@@ -34490,10 +34486,10 @@
     </row>
     <row r="261" hidden="true">
       <c r="A261" t="s" s="2">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B261" t="s" s="2">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" t="s" s="2">
@@ -34608,13 +34604,13 @@
     </row>
     <row r="262" hidden="true">
       <c r="A262" t="s" s="2">
+        <v>840</v>
+      </c>
+      <c r="B262" t="s" s="2">
+        <v>781</v>
+      </c>
+      <c r="C262" t="s" s="2">
         <v>841</v>
-      </c>
-      <c r="B262" t="s" s="2">
-        <v>782</v>
-      </c>
-      <c r="C262" t="s" s="2">
-        <v>842</v>
       </c>
       <c r="D262" t="s" s="2">
         <v>79</v>
@@ -34639,7 +34635,7 @@
         <v>112</v>
       </c>
       <c r="L262" t="s" s="2">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="M262" t="s" s="2">
         <v>206</v>
@@ -34728,10 +34724,10 @@
     </row>
     <row r="263" hidden="true">
       <c r="A263" t="s" s="2">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B263" t="s" s="2">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" t="s" s="2">
@@ -34846,10 +34842,10 @@
     </row>
     <row r="264" hidden="true">
       <c r="A264" t="s" s="2">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B264" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" t="s" s="2">
@@ -34964,10 +34960,10 @@
     </row>
     <row r="265" hidden="true">
       <c r="A265" t="s" s="2">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B265" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" t="s" s="2">
@@ -35007,7 +35003,7 @@
       </c>
       <c r="Q265" s="2"/>
       <c r="R265" t="s" s="2">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="S265" t="s" s="2">
         <v>79</v>
@@ -35084,10 +35080,10 @@
     </row>
     <row r="266" hidden="true">
       <c r="A266" t="s" s="2">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B266" t="s" s="2">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" t="s" s="2">
@@ -35202,10 +35198,10 @@
     </row>
     <row r="267" hidden="true">
       <c r="A267" t="s" s="2">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B267" t="s" s="2">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" t="s" s="2">
@@ -35245,7 +35241,7 @@
       </c>
       <c r="Q267" s="2"/>
       <c r="R267" t="s" s="2">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="S267" t="s" s="2">
         <v>79</v>
@@ -35322,10 +35318,10 @@
     </row>
     <row r="268" hidden="true">
       <c r="A268" t="s" s="2">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B268" t="s" s="2">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" t="s" s="2">
@@ -35348,7 +35344,7 @@
         <v>79</v>
       </c>
       <c r="K268" t="s" s="2">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="L268" t="s" s="2">
         <v>235</v>
@@ -35440,10 +35436,10 @@
     </row>
     <row r="269" hidden="true">
       <c r="A269" t="s" s="2">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B269" t="s" s="2">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" t="s" s="2">
@@ -35469,10 +35465,10 @@
         <v>180</v>
       </c>
       <c r="L269" t="s" s="2">
+        <v>732</v>
+      </c>
+      <c r="M269" t="s" s="2">
         <v>733</v>
-      </c>
-      <c r="M269" t="s" s="2">
-        <v>734</v>
       </c>
       <c r="N269" s="2"/>
       <c r="O269" s="2"/>
@@ -35484,7 +35480,7 @@
         <v>79</v>
       </c>
       <c r="S269" t="s" s="2">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="T269" t="s" s="2">
         <v>79</v>
@@ -35502,37 +35498,37 @@
         <v>325</v>
       </c>
       <c r="Y269" t="s" s="2">
+        <v>734</v>
+      </c>
+      <c r="Z269" t="s" s="2">
         <v>735</v>
       </c>
-      <c r="Z269" t="s" s="2">
+      <c r="AA269" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB269" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC269" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD269" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE269" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF269" t="s" s="2">
         <v>736</v>
       </c>
-      <c r="AA269" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AB269" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AC269" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AD269" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AE269" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF269" t="s" s="2">
+      <c r="AG269" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH269" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI269" t="s" s="2">
         <v>737</v>
-      </c>
-      <c r="AG269" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH269" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AI269" t="s" s="2">
-        <v>738</v>
       </c>
       <c r="AJ269" t="s" s="2">
         <v>103</v>
@@ -35544,13 +35540,13 @@
         <v>79</v>
       </c>
       <c r="AM269" t="s" s="2">
+        <v>738</v>
+      </c>
+      <c r="AN269" t="s" s="2">
         <v>739</v>
       </c>
-      <c r="AN269" t="s" s="2">
+      <c r="AO269" t="s" s="2">
         <v>740</v>
-      </c>
-      <c r="AO269" t="s" s="2">
-        <v>741</v>
       </c>
       <c r="AP269" t="s" s="2">
         <v>79</v>
@@ -35558,10 +35554,10 @@
     </row>
     <row r="270" hidden="true">
       <c r="A270" t="s" s="2">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B270" t="s" s="2">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" t="s" s="2">
@@ -35587,16 +35583,16 @@
         <v>105</v>
       </c>
       <c r="L270" t="s" s="2">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M270" t="s" s="2">
+        <v>743</v>
+      </c>
+      <c r="N270" t="s" s="2">
         <v>744</v>
       </c>
-      <c r="N270" t="s" s="2">
+      <c r="O270" t="s" s="2">
         <v>745</v>
-      </c>
-      <c r="O270" t="s" s="2">
-        <v>746</v>
       </c>
       <c r="P270" t="s" s="2">
         <v>79</v>
@@ -35645,7 +35641,7 @@
         <v>79</v>
       </c>
       <c r="AF270" t="s" s="2">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AG270" t="s" s="2">
         <v>80</v>
@@ -35666,10 +35662,10 @@
         <v>79</v>
       </c>
       <c r="AM270" t="s" s="2">
+        <v>747</v>
+      </c>
+      <c r="AN270" t="s" s="2">
         <v>748</v>
-      </c>
-      <c r="AN270" t="s" s="2">
-        <v>749</v>
       </c>
       <c r="AO270" t="s" s="2">
         <v>358</v>
@@ -35680,10 +35676,10 @@
     </row>
     <row r="271" hidden="true">
       <c r="A271" t="s" s="2">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B271" t="s" s="2">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" t="s" s="2">
@@ -35709,16 +35705,16 @@
         <v>180</v>
       </c>
       <c r="L271" t="s" s="2">
+        <v>750</v>
+      </c>
+      <c r="M271" t="s" s="2">
         <v>751</v>
       </c>
-      <c r="M271" t="s" s="2">
-        <v>752</v>
-      </c>
       <c r="N271" t="s" s="2">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="O271" t="s" s="2">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="P271" t="s" s="2">
         <v>79</v>
@@ -35746,28 +35742,28 @@
         <v>325</v>
       </c>
       <c r="Y271" t="s" s="2">
+        <v>754</v>
+      </c>
+      <c r="Z271" t="s" s="2">
         <v>755</v>
       </c>
-      <c r="Z271" t="s" s="2">
+      <c r="AA271" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB271" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC271" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD271" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE271" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF271" t="s" s="2">
         <v>756</v>
-      </c>
-      <c r="AA271" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AB271" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AC271" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AD271" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AE271" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF271" t="s" s="2">
-        <v>757</v>
       </c>
       <c r="AG271" t="s" s="2">
         <v>80</v>
@@ -35788,13 +35784,13 @@
         <v>79</v>
       </c>
       <c r="AM271" t="s" s="2">
+        <v>757</v>
+      </c>
+      <c r="AN271" t="s" s="2">
         <v>758</v>
       </c>
-      <c r="AN271" t="s" s="2">
+      <c r="AO271" t="s" s="2">
         <v>759</v>
-      </c>
-      <c r="AO271" t="s" s="2">
-        <v>760</v>
       </c>
       <c r="AP271" t="s" s="2">
         <v>79</v>
@@ -35802,10 +35798,10 @@
     </row>
     <row r="272" hidden="true">
       <c r="A272" t="s" s="2">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B272" t="s" s="2">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" t="s" s="2">
@@ -35828,16 +35824,16 @@
         <v>92</v>
       </c>
       <c r="K272" t="s" s="2">
+        <v>761</v>
+      </c>
+      <c r="L272" t="s" s="2">
         <v>762</v>
       </c>
-      <c r="L272" t="s" s="2">
+      <c r="M272" t="s" s="2">
         <v>763</v>
       </c>
-      <c r="M272" t="s" s="2">
+      <c r="N272" t="s" s="2">
         <v>764</v>
-      </c>
-      <c r="N272" t="s" s="2">
-        <v>765</v>
       </c>
       <c r="O272" s="2"/>
       <c r="P272" t="s" s="2">
@@ -35887,7 +35883,7 @@
         <v>79</v>
       </c>
       <c r="AF272" t="s" s="2">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AG272" t="s" s="2">
         <v>80</v>
@@ -35922,10 +35918,10 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B273" t="s" s="2">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" t="s" s="2">
@@ -35951,10 +35947,10 @@
         <v>234</v>
       </c>
       <c r="L273" t="s" s="2">
+        <v>767</v>
+      </c>
+      <c r="M273" t="s" s="2">
         <v>768</v>
-      </c>
-      <c r="M273" t="s" s="2">
-        <v>769</v>
       </c>
       <c r="N273" s="2"/>
       <c r="O273" s="2"/>
@@ -36005,7 +36001,7 @@
         <v>79</v>
       </c>
       <c r="AF273" t="s" s="2">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AG273" t="s" s="2">
         <v>80</v>
@@ -36029,7 +36025,7 @@
         <v>203</v>
       </c>
       <c r="AN273" t="s" s="2">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="AO273" t="s" s="2">
         <v>365</v>
@@ -36040,10 +36036,10 @@
     </row>
     <row r="274" hidden="true">
       <c r="A274" t="s" s="2">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B274" t="s" s="2">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" t="s" s="2">
@@ -36066,19 +36062,19 @@
         <v>79</v>
       </c>
       <c r="K274" t="s" s="2">
+        <v>860</v>
+      </c>
+      <c r="L274" t="s" s="2">
         <v>861</v>
       </c>
-      <c r="L274" t="s" s="2">
+      <c r="M274" t="s" s="2">
         <v>862</v>
       </c>
-      <c r="M274" t="s" s="2">
+      <c r="N274" t="s" s="2">
         <v>863</v>
       </c>
-      <c r="N274" t="s" s="2">
+      <c r="O274" t="s" s="2">
         <v>864</v>
-      </c>
-      <c r="O274" t="s" s="2">
-        <v>865</v>
       </c>
       <c r="P274" t="s" s="2">
         <v>79</v>
@@ -36127,7 +36123,7 @@
         <v>79</v>
       </c>
       <c r="AF274" t="s" s="2">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="AG274" t="s" s="2">
         <v>80</v>
@@ -36139,22 +36135,22 @@
         <v>212</v>
       </c>
       <c r="AJ274" t="s" s="2">
+        <v>865</v>
+      </c>
+      <c r="AK274" t="s" s="2">
         <v>866</v>
       </c>
-      <c r="AK274" t="s" s="2">
+      <c r="AL274" t="s" s="2">
         <v>867</v>
       </c>
-      <c r="AL274" t="s" s="2">
+      <c r="AM274" t="s" s="2">
         <v>868</v>
       </c>
-      <c r="AM274" t="s" s="2">
+      <c r="AN274" t="s" s="2">
         <v>869</v>
       </c>
-      <c r="AN274" t="s" s="2">
+      <c r="AO274" t="s" s="2">
         <v>870</v>
-      </c>
-      <c r="AO274" t="s" s="2">
-        <v>871</v>
       </c>
       <c r="AP274" t="s" s="2">
         <v>79</v>
@@ -36162,10 +36158,10 @@
     </row>
     <row r="275" hidden="true">
       <c r="A275" t="s" s="2">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B275" t="s" s="2">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" t="s" s="2">
@@ -36188,17 +36184,17 @@
         <v>92</v>
       </c>
       <c r="K275" t="s" s="2">
+        <v>872</v>
+      </c>
+      <c r="L275" t="s" s="2">
         <v>873</v>
       </c>
-      <c r="L275" t="s" s="2">
+      <c r="M275" t="s" s="2">
         <v>874</v>
-      </c>
-      <c r="M275" t="s" s="2">
-        <v>875</v>
       </c>
       <c r="N275" s="2"/>
       <c r="O275" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="P275" t="s" s="2">
         <v>79</v>
@@ -36247,7 +36243,7 @@
         <v>79</v>
       </c>
       <c r="AF275" t="s" s="2">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="AG275" t="s" s="2">
         <v>80</v>
@@ -36271,7 +36267,7 @@
         <v>547</v>
       </c>
       <c r="AN275" t="s" s="2">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="AO275" t="s" s="2">
         <v>109</v>
@@ -36282,10 +36278,10 @@
     </row>
     <row r="276" hidden="true">
       <c r="A276" t="s" s="2">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B276" t="s" s="2">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" t="s" s="2">
@@ -36400,10 +36396,10 @@
     </row>
     <row r="277" hidden="true">
       <c r="A277" t="s" s="2">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B277" t="s" s="2">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" t="s" s="2">
@@ -36520,10 +36516,10 @@
     </row>
     <row r="278" hidden="true">
       <c r="A278" t="s" s="2">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B278" t="s" s="2">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" t="s" s="2">
@@ -36549,13 +36545,13 @@
         <v>105</v>
       </c>
       <c r="L278" t="s" s="2">
+        <v>880</v>
+      </c>
+      <c r="M278" t="s" s="2">
         <v>881</v>
       </c>
-      <c r="M278" t="s" s="2">
+      <c r="N278" t="s" s="2">
         <v>882</v>
-      </c>
-      <c r="N278" t="s" s="2">
-        <v>883</v>
       </c>
       <c r="O278" s="2"/>
       <c r="P278" t="s" s="2">
@@ -36605,16 +36601,16 @@
         <v>79</v>
       </c>
       <c r="AF278" t="s" s="2">
+        <v>883</v>
+      </c>
+      <c r="AG278" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH278" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI278" t="s" s="2">
         <v>884</v>
-      </c>
-      <c r="AG278" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH278" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AI278" t="s" s="2">
-        <v>885</v>
       </c>
       <c r="AJ278" t="s" s="2">
         <v>103</v>
@@ -36640,10 +36636,10 @@
     </row>
     <row r="279" hidden="true">
       <c r="A279" t="s" s="2">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B279" t="s" s="2">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" t="s" s="2">
@@ -36669,13 +36665,13 @@
         <v>138</v>
       </c>
       <c r="L279" t="s" s="2">
+        <v>886</v>
+      </c>
+      <c r="M279" t="s" s="2">
         <v>887</v>
       </c>
-      <c r="M279" t="s" s="2">
+      <c r="N279" t="s" s="2">
         <v>888</v>
-      </c>
-      <c r="N279" t="s" s="2">
-        <v>889</v>
       </c>
       <c r="O279" s="2"/>
       <c r="P279" t="s" s="2">
@@ -36723,7 +36719,7 @@
         <v>79</v>
       </c>
       <c r="AF279" t="s" s="2">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="AG279" t="s" s="2">
         <v>80</v>
@@ -36758,10 +36754,10 @@
     </row>
     <row r="280" hidden="true">
       <c r="A280" t="s" s="2">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B280" t="s" s="2">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" t="s" s="2">
@@ -36787,13 +36783,13 @@
         <v>307</v>
       </c>
       <c r="L280" t="s" s="2">
+        <v>891</v>
+      </c>
+      <c r="M280" t="s" s="2">
         <v>892</v>
       </c>
-      <c r="M280" t="s" s="2">
+      <c r="N280" t="s" s="2">
         <v>893</v>
-      </c>
-      <c r="N280" t="s" s="2">
-        <v>894</v>
       </c>
       <c r="O280" s="2"/>
       <c r="P280" t="s" s="2">
@@ -36843,7 +36839,7 @@
         <v>79</v>
       </c>
       <c r="AF280" t="s" s="2">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AG280" t="s" s="2">
         <v>80</v>
@@ -36867,7 +36863,7 @@
         <v>79</v>
       </c>
       <c r="AN280" t="s" s="2">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="AO280" t="s" s="2">
         <v>79</v>
@@ -36878,10 +36874,10 @@
     </row>
     <row r="281" hidden="true">
       <c r="A281" t="s" s="2">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B281" t="s" s="2">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" t="s" s="2">
@@ -36907,13 +36903,13 @@
         <v>105</v>
       </c>
       <c r="L281" t="s" s="2">
+        <v>897</v>
+      </c>
+      <c r="M281" t="s" s="2">
         <v>898</v>
       </c>
-      <c r="M281" t="s" s="2">
+      <c r="N281" t="s" s="2">
         <v>899</v>
-      </c>
-      <c r="N281" t="s" s="2">
-        <v>900</v>
       </c>
       <c r="O281" s="2"/>
       <c r="P281" t="s" s="2">
@@ -36963,7 +36959,7 @@
         <v>79</v>
       </c>
       <c r="AF281" t="s" s="2">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AG281" t="s" s="2">
         <v>80</v>
@@ -36998,10 +36994,10 @@
     </row>
     <row r="282" hidden="true">
       <c r="A282" t="s" s="2">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B282" t="s" s="2">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" t="s" s="2">
@@ -37024,19 +37020,19 @@
         <v>79</v>
       </c>
       <c r="K282" t="s" s="2">
+        <v>902</v>
+      </c>
+      <c r="L282" t="s" s="2">
         <v>903</v>
       </c>
-      <c r="L282" t="s" s="2">
+      <c r="M282" t="s" s="2">
         <v>904</v>
       </c>
-      <c r="M282" t="s" s="2">
+      <c r="N282" t="s" s="2">
         <v>905</v>
       </c>
-      <c r="N282" t="s" s="2">
+      <c r="O282" t="s" s="2">
         <v>906</v>
-      </c>
-      <c r="O282" t="s" s="2">
-        <v>907</v>
       </c>
       <c r="P282" t="s" s="2">
         <v>79</v>
@@ -37085,7 +37081,7 @@
         <v>79</v>
       </c>
       <c r="AF282" t="s" s="2">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AG282" t="s" s="2">
         <v>80</v>
@@ -37109,7 +37105,7 @@
         <v>79</v>
       </c>
       <c r="AN282" t="s" s="2">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="AO282" t="s" s="2">
         <v>79</v>
@@ -37120,10 +37116,10 @@
     </row>
     <row r="283" hidden="true">
       <c r="A283" t="s" s="2">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B283" t="s" s="2">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" t="s" s="2">
@@ -37238,10 +37234,10 @@
     </row>
     <row r="284" hidden="true">
       <c r="A284" t="s" s="2">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B284" t="s" s="2">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" t="s" s="2">
@@ -37358,14 +37354,14 @@
     </row>
     <row r="285" hidden="true">
       <c r="A285" t="s" s="2">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B285" t="s" s="2">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" t="s" s="2">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E285" s="2"/>
       <c r="F285" t="s" s="2">
@@ -37387,10 +37383,10 @@
         <v>112</v>
       </c>
       <c r="L285" t="s" s="2">
+        <v>912</v>
+      </c>
+      <c r="M285" t="s" s="2">
         <v>913</v>
-      </c>
-      <c r="M285" t="s" s="2">
-        <v>914</v>
       </c>
       <c r="N285" t="s" s="2">
         <v>115</v>
@@ -37445,7 +37441,7 @@
         <v>79</v>
       </c>
       <c r="AF285" t="s" s="2">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="AG285" t="s" s="2">
         <v>80</v>
@@ -37480,10 +37476,10 @@
     </row>
     <row r="286" hidden="true">
       <c r="A286" t="s" s="2">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B286" t="s" s="2">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" t="s" s="2">
@@ -37509,14 +37505,14 @@
         <v>331</v>
       </c>
       <c r="L286" t="s" s="2">
+        <v>916</v>
+      </c>
+      <c r="M286" t="s" s="2">
         <v>917</v>
-      </c>
-      <c r="M286" t="s" s="2">
-        <v>918</v>
       </c>
       <c r="N286" s="2"/>
       <c r="O286" t="s" s="2">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="P286" t="s" s="2">
         <v>79</v>
@@ -37544,11 +37540,11 @@
         <v>162</v>
       </c>
       <c r="Y286" t="s" s="2">
+        <v>919</v>
+      </c>
+      <c r="Z286" t="s" s="2">
         <v>920</v>
       </c>
-      <c r="Z286" t="s" s="2">
-        <v>921</v>
-      </c>
       <c r="AA286" t="s" s="2">
         <v>79</v>
       </c>
@@ -37565,7 +37561,7 @@
         <v>79</v>
       </c>
       <c r="AF286" t="s" s="2">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="AG286" t="s" s="2">
         <v>80</v>
@@ -37589,7 +37585,7 @@
         <v>79</v>
       </c>
       <c r="AN286" t="s" s="2">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AO286" t="s" s="2">
         <v>79</v>
@@ -37600,10 +37596,10 @@
     </row>
     <row r="287" hidden="true">
       <c r="A287" t="s" s="2">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B287" t="s" s="2">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" t="s" s="2">
@@ -37626,17 +37622,17 @@
         <v>79</v>
       </c>
       <c r="K287" t="s" s="2">
+        <v>923</v>
+      </c>
+      <c r="L287" t="s" s="2">
         <v>924</v>
       </c>
-      <c r="L287" t="s" s="2">
+      <c r="M287" t="s" s="2">
         <v>925</v>
-      </c>
-      <c r="M287" t="s" s="2">
-        <v>926</v>
       </c>
       <c r="N287" s="2"/>
       <c r="O287" t="s" s="2">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="P287" t="s" s="2">
         <v>79</v>
@@ -37685,7 +37681,7 @@
         <v>79</v>
       </c>
       <c r="AF287" t="s" s="2">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AG287" t="s" s="2">
         <v>80</v>
@@ -37706,10 +37702,10 @@
         <v>79</v>
       </c>
       <c r="AM287" t="s" s="2">
+        <v>927</v>
+      </c>
+      <c r="AN287" t="s" s="2">
         <v>928</v>
-      </c>
-      <c r="AN287" t="s" s="2">
-        <v>929</v>
       </c>
       <c r="AO287" t="s" s="2">
         <v>79</v>
@@ -37720,10 +37716,10 @@
     </row>
     <row r="288" hidden="true">
       <c r="A288" t="s" s="2">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B288" t="s" s="2">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" t="s" s="2">
@@ -37749,14 +37745,14 @@
         <v>713</v>
       </c>
       <c r="L288" t="s" s="2">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="M288" t="s" s="2">
         <v>715</v>
       </c>
       <c r="N288" s="2"/>
       <c r="O288" t="s" s="2">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="P288" t="s" s="2">
         <v>79</v>
@@ -37805,7 +37801,7 @@
         <v>79</v>
       </c>
       <c r="AF288" t="s" s="2">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AG288" t="s" s="2">
         <v>80</v>
@@ -37817,7 +37813,7 @@
         <v>212</v>
       </c>
       <c r="AJ288" t="s" s="2">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AK288" t="s" s="2">
         <v>79</v>
@@ -37826,13 +37822,13 @@
         <v>79</v>
       </c>
       <c r="AM288" t="s" s="2">
+        <v>721</v>
+      </c>
+      <c r="AN288" t="s" s="2">
         <v>722</v>
       </c>
-      <c r="AN288" t="s" s="2">
+      <c r="AO288" t="s" s="2">
         <v>723</v>
-      </c>
-      <c r="AO288" t="s" s="2">
-        <v>724</v>
       </c>
       <c r="AP288" t="s" s="2">
         <v>79</v>
@@ -37840,10 +37836,10 @@
     </row>
     <row r="289" hidden="true">
       <c r="A289" t="s" s="2">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B289" t="s" s="2">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" t="s" s="2">
@@ -37866,19 +37862,19 @@
         <v>79</v>
       </c>
       <c r="K289" t="s" s="2">
+        <v>933</v>
+      </c>
+      <c r="L289" t="s" s="2">
         <v>934</v>
       </c>
-      <c r="L289" t="s" s="2">
+      <c r="M289" t="s" s="2">
+        <v>862</v>
+      </c>
+      <c r="N289" t="s" s="2">
+        <v>863</v>
+      </c>
+      <c r="O289" t="s" s="2">
         <v>935</v>
-      </c>
-      <c r="M289" t="s" s="2">
-        <v>863</v>
-      </c>
-      <c r="N289" t="s" s="2">
-        <v>864</v>
-      </c>
-      <c r="O289" t="s" s="2">
-        <v>936</v>
       </c>
       <c r="P289" t="s" s="2">
         <v>79</v>
@@ -37927,7 +37923,7 @@
         <v>79</v>
       </c>
       <c r="AF289" t="s" s="2">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AG289" t="s" s="2">
         <v>80</v>
@@ -37948,13 +37944,13 @@
         <v>79</v>
       </c>
       <c r="AM289" t="s" s="2">
+        <v>868</v>
+      </c>
+      <c r="AN289" t="s" s="2">
         <v>869</v>
       </c>
-      <c r="AN289" t="s" s="2">
+      <c r="AO289" t="s" s="2">
         <v>870</v>
-      </c>
-      <c r="AO289" t="s" s="2">
-        <v>871</v>
       </c>
       <c r="AP289" t="s" s="2">
         <v>79</v>
@@ -37962,10 +37958,10 @@
     </row>
     <row r="290" hidden="true">
       <c r="A290" t="s" s="2">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B290" t="s" s="2">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" t="s" s="2">
@@ -37988,17 +37984,17 @@
         <v>79</v>
       </c>
       <c r="K290" t="s" s="2">
+        <v>937</v>
+      </c>
+      <c r="L290" t="s" s="2">
         <v>938</v>
       </c>
-      <c r="L290" t="s" s="2">
+      <c r="M290" t="s" s="2">
         <v>939</v>
-      </c>
-      <c r="M290" t="s" s="2">
-        <v>940</v>
       </c>
       <c r="N290" s="2"/>
       <c r="O290" t="s" s="2">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="P290" t="s" s="2">
         <v>79</v>
@@ -38047,7 +38043,7 @@
         <v>79</v>
       </c>
       <c r="AF290" t="s" s="2">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AG290" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
test new discr 4c99e90a8405735b7a6820decf06490e24f106f4
</commit_message>
<xml_diff>
--- a/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-organization.xlsx
+++ b/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-organization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11037" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11037" uniqueCount="942">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-11T14:48:45+00:00</t>
+    <t>2024-10-12T09:26:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2245,6 +2245,10 @@
   </si>
   <si>
     <t>Human contact for the organization.</t>
+  </si>
+  <si>
+    <t>pattern:system}
+pattern:extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-contact-point-email-type').value}</t>
   </si>
   <si>
     <t>cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}
@@ -3300,7 +3304,7 @@
     <col min="25" max="25" width="98.61328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="108.3828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="96.68359375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -28727,7 +28731,7 @@
         <v>79</v>
       </c>
       <c r="AB212" t="s" s="2">
-        <v>558</v>
+        <v>718</v>
       </c>
       <c r="AC212" s="2"/>
       <c r="AD212" t="s" s="2">
@@ -28749,22 +28753,22 @@
         <v>212</v>
       </c>
       <c r="AJ212" t="s" s="2">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="AK212" t="s" s="2">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="AL212" t="s" s="2">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="AM212" t="s" s="2">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="AN212" t="s" s="2">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="AO212" t="s" s="2">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="AP212" t="s" s="2">
         <v>79</v>
@@ -28772,10 +28776,10 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B213" t="s" s="2">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" t="s" s="2">
@@ -28890,10 +28894,10 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B214" t="s" s="2">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" t="s" s="2">
@@ -29010,13 +29014,13 @@
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
+        <v>727</v>
+      </c>
+      <c r="B215" t="s" s="2">
         <v>726</v>
       </c>
-      <c r="B215" t="s" s="2">
-        <v>725</v>
-      </c>
       <c r="C215" t="s" s="2">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="D215" t="s" s="2">
         <v>79</v>
@@ -29038,13 +29042,13 @@
         <v>79</v>
       </c>
       <c r="K215" t="s" s="2">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="L215" t="s" s="2">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="M215" t="s" s="2">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="N215" s="2"/>
       <c r="O215" s="2"/>
@@ -29130,10 +29134,10 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B216" t="s" s="2">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" t="s" s="2">
@@ -29159,10 +29163,10 @@
         <v>180</v>
       </c>
       <c r="L216" t="s" s="2">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="M216" t="s" s="2">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="N216" s="2"/>
       <c r="O216" s="2"/>
@@ -29192,10 +29196,10 @@
         <v>325</v>
       </c>
       <c r="Y216" t="s" s="2">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="Z216" t="s" s="2">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="AA216" t="s" s="2">
         <v>79</v>
@@ -29213,7 +29217,7 @@
         <v>79</v>
       </c>
       <c r="AF216" t="s" s="2">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="AG216" t="s" s="2">
         <v>80</v>
@@ -29222,7 +29226,7 @@
         <v>91</v>
       </c>
       <c r="AI216" t="s" s="2">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="AJ216" t="s" s="2">
         <v>103</v>
@@ -29234,13 +29238,13 @@
         <v>79</v>
       </c>
       <c r="AM216" t="s" s="2">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="AN216" t="s" s="2">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="AO216" t="s" s="2">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="AP216" t="s" s="2">
         <v>79</v>
@@ -29248,10 +29252,10 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B217" t="s" s="2">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" t="s" s="2">
@@ -29277,16 +29281,16 @@
         <v>105</v>
       </c>
       <c r="L217" t="s" s="2">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="M217" t="s" s="2">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="N217" t="s" s="2">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="O217" t="s" s="2">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="P217" t="s" s="2">
         <v>79</v>
@@ -29335,7 +29339,7 @@
         <v>79</v>
       </c>
       <c r="AF217" t="s" s="2">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="AG217" t="s" s="2">
         <v>80</v>
@@ -29356,10 +29360,10 @@
         <v>79</v>
       </c>
       <c r="AM217" t="s" s="2">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="AN217" t="s" s="2">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="AO217" t="s" s="2">
         <v>358</v>
@@ -29370,10 +29374,10 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B218" t="s" s="2">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" t="s" s="2">
@@ -29399,16 +29403,16 @@
         <v>180</v>
       </c>
       <c r="L218" t="s" s="2">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="M218" t="s" s="2">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="N218" t="s" s="2">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="O218" t="s" s="2">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="P218" t="s" s="2">
         <v>79</v>
@@ -29436,10 +29440,10 @@
         <v>325</v>
       </c>
       <c r="Y218" t="s" s="2">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="Z218" t="s" s="2">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="AA218" t="s" s="2">
         <v>79</v>
@@ -29457,7 +29461,7 @@
         <v>79</v>
       </c>
       <c r="AF218" t="s" s="2">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="AG218" t="s" s="2">
         <v>80</v>
@@ -29478,13 +29482,13 @@
         <v>79</v>
       </c>
       <c r="AM218" t="s" s="2">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="AN218" t="s" s="2">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="AO218" t="s" s="2">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="AP218" t="s" s="2">
         <v>79</v>
@@ -29492,10 +29496,10 @@
     </row>
     <row r="219" hidden="true">
       <c r="A219" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B219" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" t="s" s="2">
@@ -29518,16 +29522,16 @@
         <v>92</v>
       </c>
       <c r="K219" t="s" s="2">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="L219" t="s" s="2">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="M219" t="s" s="2">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="N219" t="s" s="2">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="O219" s="2"/>
       <c r="P219" t="s" s="2">
@@ -29577,7 +29581,7 @@
         <v>79</v>
       </c>
       <c r="AF219" t="s" s="2">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="AG219" t="s" s="2">
         <v>80</v>
@@ -29612,10 +29616,10 @@
     </row>
     <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B220" t="s" s="2">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" t="s" s="2">
@@ -29641,10 +29645,10 @@
         <v>234</v>
       </c>
       <c r="L220" t="s" s="2">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="M220" t="s" s="2">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="N220" s="2"/>
       <c r="O220" s="2"/>
@@ -29695,7 +29699,7 @@
         <v>79</v>
       </c>
       <c r="AF220" t="s" s="2">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AG220" t="s" s="2">
         <v>80</v>
@@ -29719,7 +29723,7 @@
         <v>203</v>
       </c>
       <c r="AN220" t="s" s="2">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AO220" t="s" s="2">
         <v>365</v>
@@ -29730,13 +29734,13 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B221" t="s" s="2">
         <v>712</v>
       </c>
       <c r="C221" t="s" s="2">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="D221" t="s" s="2">
         <v>79</v>
@@ -29758,10 +29762,10 @@
         <v>79</v>
       </c>
       <c r="K221" t="s" s="2">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="L221" t="s" s="2">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="M221" t="s" s="2">
         <v>715</v>
@@ -29831,7 +29835,7 @@
         <v>212</v>
       </c>
       <c r="AJ221" t="s" s="2">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="AK221" t="s" s="2">
         <v>79</v>
@@ -29840,13 +29844,13 @@
         <v>79</v>
       </c>
       <c r="AM221" t="s" s="2">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="AN221" t="s" s="2">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="AO221" t="s" s="2">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="AP221" t="s" s="2">
         <v>79</v>
@@ -29854,10 +29858,10 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B222" t="s" s="2">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" t="s" s="2">
@@ -29972,10 +29976,10 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B223" t="s" s="2">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" t="s" s="2">
@@ -30092,13 +30096,13 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B224" t="s" s="2">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C224" t="s" s="2">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="D224" t="s" s="2">
         <v>79</v>
@@ -30120,13 +30124,13 @@
         <v>79</v>
       </c>
       <c r="K224" t="s" s="2">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="L224" t="s" s="2">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="M224" t="s" s="2">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="N224" s="2"/>
       <c r="O224" s="2"/>
@@ -30212,10 +30216,10 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B225" t="s" s="2">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" t="s" s="2">
@@ -30330,10 +30334,10 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B226" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" t="s" s="2">
@@ -30448,10 +30452,10 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B227" t="s" s="2">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" t="s" s="2">
@@ -30491,7 +30495,7 @@
       </c>
       <c r="Q227" s="2"/>
       <c r="R227" t="s" s="2">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="S227" t="s" s="2">
         <v>79</v>
@@ -30568,10 +30572,10 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B228" t="s" s="2">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" t="s" s="2">
@@ -30612,7 +30616,7 @@
         <v>79</v>
       </c>
       <c r="S228" t="s" s="2">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="T228" t="s" s="2">
         <v>79</v>
@@ -30631,7 +30635,7 @@
       </c>
       <c r="Y228" s="2"/>
       <c r="Z228" t="s" s="2">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="AA228" t="s" s="2">
         <v>79</v>
@@ -30684,13 +30688,13 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B229" t="s" s="2">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C229" t="s" s="2">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D229" t="s" s="2">
         <v>79</v>
@@ -30712,13 +30716,13 @@
         <v>79</v>
       </c>
       <c r="K229" t="s" s="2">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="L229" t="s" s="2">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="M229" t="s" s="2">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="N229" s="2"/>
       <c r="O229" s="2"/>
@@ -30804,10 +30808,10 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B230" t="s" s="2">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" t="s" s="2">
@@ -30922,10 +30926,10 @@
     </row>
     <row r="231" hidden="true">
       <c r="A231" t="s" s="2">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B231" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" t="s" s="2">
@@ -31042,13 +31046,13 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B232" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C232" t="s" s="2">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D232" t="s" s="2">
         <v>79</v>
@@ -31073,7 +31077,7 @@
         <v>112</v>
       </c>
       <c r="L232" t="s" s="2">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="M232" t="s" s="2">
         <v>206</v>
@@ -31162,10 +31166,10 @@
     </row>
     <row r="233" hidden="true">
       <c r="A233" t="s" s="2">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B233" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" t="s" s="2">
@@ -31280,10 +31284,10 @@
     </row>
     <row r="234" hidden="true">
       <c r="A234" t="s" s="2">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B234" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" t="s" s="2">
@@ -31398,10 +31402,10 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B235" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" t="s" s="2">
@@ -31441,7 +31445,7 @@
       </c>
       <c r="Q235" s="2"/>
       <c r="R235" t="s" s="2">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="S235" t="s" s="2">
         <v>79</v>
@@ -31518,10 +31522,10 @@
     </row>
     <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B236" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" t="s" s="2">
@@ -31581,7 +31585,7 @@
       </c>
       <c r="Y236" s="2"/>
       <c r="Z236" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="AA236" t="s" s="2">
         <v>79</v>
@@ -31634,10 +31638,10 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B237" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C237" t="s" s="2">
         <v>214</v>
@@ -31665,7 +31669,7 @@
         <v>112</v>
       </c>
       <c r="L237" t="s" s="2">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="M237" t="s" s="2">
         <v>206</v>
@@ -31754,10 +31758,10 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B238" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" t="s" s="2">
@@ -31872,10 +31876,10 @@
     </row>
     <row r="239" hidden="true">
       <c r="A239" t="s" s="2">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B239" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" t="s" s="2">
@@ -31990,10 +31994,10 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B240" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" t="s" s="2">
@@ -32110,10 +32114,10 @@
     </row>
     <row r="241" hidden="true">
       <c r="A241" t="s" s="2">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B241" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C241" s="2"/>
       <c r="D241" t="s" s="2">
@@ -32228,13 +32232,13 @@
     </row>
     <row r="242" hidden="true">
       <c r="A242" t="s" s="2">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B242" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C242" t="s" s="2">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D242" t="s" s="2">
         <v>79</v>
@@ -32348,10 +32352,10 @@
     </row>
     <row r="243" hidden="true">
       <c r="A243" t="s" s="2">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B243" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" t="s" s="2">
@@ -32466,10 +32470,10 @@
     </row>
     <row r="244" hidden="true">
       <c r="A244" t="s" s="2">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B244" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" t="s" s="2">
@@ -32584,10 +32588,10 @@
     </row>
     <row r="245" hidden="true">
       <c r="A245" t="s" s="2">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B245" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" t="s" s="2">
@@ -32627,7 +32631,7 @@
       </c>
       <c r="Q245" s="2"/>
       <c r="R245" t="s" s="2">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="S245" t="s" s="2">
         <v>79</v>
@@ -32704,10 +32708,10 @@
     </row>
     <row r="246" hidden="true">
       <c r="A246" t="s" s="2">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B246" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" t="s" s="2">
@@ -32822,13 +32826,13 @@
     </row>
     <row r="247" hidden="true">
       <c r="A247" t="s" s="2">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B247" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C247" t="s" s="2">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D247" t="s" s="2">
         <v>79</v>
@@ -32853,7 +32857,7 @@
         <v>112</v>
       </c>
       <c r="L247" t="s" s="2">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="M247" t="s" s="2">
         <v>206</v>
@@ -32942,10 +32946,10 @@
     </row>
     <row r="248" hidden="true">
       <c r="A248" t="s" s="2">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B248" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" t="s" s="2">
@@ -33060,10 +33064,10 @@
     </row>
     <row r="249" hidden="true">
       <c r="A249" t="s" s="2">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B249" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" t="s" s="2">
@@ -33178,10 +33182,10 @@
     </row>
     <row r="250" hidden="true">
       <c r="A250" t="s" s="2">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B250" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" t="s" s="2">
@@ -33221,7 +33225,7 @@
       </c>
       <c r="Q250" s="2"/>
       <c r="R250" t="s" s="2">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="S250" t="s" s="2">
         <v>79</v>
@@ -33298,10 +33302,10 @@
     </row>
     <row r="251" hidden="true">
       <c r="A251" t="s" s="2">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B251" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" t="s" s="2">
@@ -33416,13 +33420,13 @@
     </row>
     <row r="252" hidden="true">
       <c r="A252" t="s" s="2">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B252" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C252" t="s" s="2">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D252" t="s" s="2">
         <v>79</v>
@@ -33536,10 +33540,10 @@
     </row>
     <row r="253" hidden="true">
       <c r="A253" t="s" s="2">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B253" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" t="s" s="2">
@@ -33654,10 +33658,10 @@
     </row>
     <row r="254" hidden="true">
       <c r="A254" t="s" s="2">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B254" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" t="s" s="2">
@@ -33772,10 +33776,10 @@
     </row>
     <row r="255" hidden="true">
       <c r="A255" t="s" s="2">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B255" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" t="s" s="2">
@@ -33815,7 +33819,7 @@
       </c>
       <c r="Q255" s="2"/>
       <c r="R255" t="s" s="2">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="S255" t="s" s="2">
         <v>79</v>
@@ -33892,10 +33896,10 @@
     </row>
     <row r="256" hidden="true">
       <c r="A256" t="s" s="2">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B256" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" t="s" s="2">
@@ -34010,13 +34014,13 @@
     </row>
     <row r="257" hidden="true">
       <c r="A257" t="s" s="2">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B257" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C257" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D257" t="s" s="2">
         <v>79</v>
@@ -34041,7 +34045,7 @@
         <v>112</v>
       </c>
       <c r="L257" t="s" s="2">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="M257" t="s" s="2">
         <v>206</v>
@@ -34130,10 +34134,10 @@
     </row>
     <row r="258" hidden="true">
       <c r="A258" t="s" s="2">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B258" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" t="s" s="2">
@@ -34248,10 +34252,10 @@
     </row>
     <row r="259" hidden="true">
       <c r="A259" t="s" s="2">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B259" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" t="s" s="2">
@@ -34366,10 +34370,10 @@
     </row>
     <row r="260" hidden="true">
       <c r="A260" t="s" s="2">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B260" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" t="s" s="2">
@@ -34409,7 +34413,7 @@
       </c>
       <c r="Q260" s="2"/>
       <c r="R260" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="S260" t="s" s="2">
         <v>79</v>
@@ -34486,10 +34490,10 @@
     </row>
     <row r="261" hidden="true">
       <c r="A261" t="s" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B261" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" t="s" s="2">
@@ -34604,13 +34608,13 @@
     </row>
     <row r="262" hidden="true">
       <c r="A262" t="s" s="2">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B262" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C262" t="s" s="2">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D262" t="s" s="2">
         <v>79</v>
@@ -34635,7 +34639,7 @@
         <v>112</v>
       </c>
       <c r="L262" t="s" s="2">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="M262" t="s" s="2">
         <v>206</v>
@@ -34724,10 +34728,10 @@
     </row>
     <row r="263" hidden="true">
       <c r="A263" t="s" s="2">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B263" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" t="s" s="2">
@@ -34842,10 +34846,10 @@
     </row>
     <row r="264" hidden="true">
       <c r="A264" t="s" s="2">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B264" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" t="s" s="2">
@@ -34960,10 +34964,10 @@
     </row>
     <row r="265" hidden="true">
       <c r="A265" t="s" s="2">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B265" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" t="s" s="2">
@@ -35003,7 +35007,7 @@
       </c>
       <c r="Q265" s="2"/>
       <c r="R265" t="s" s="2">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="S265" t="s" s="2">
         <v>79</v>
@@ -35080,10 +35084,10 @@
     </row>
     <row r="266" hidden="true">
       <c r="A266" t="s" s="2">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B266" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" t="s" s="2">
@@ -35198,10 +35202,10 @@
     </row>
     <row r="267" hidden="true">
       <c r="A267" t="s" s="2">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B267" t="s" s="2">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" t="s" s="2">
@@ -35241,7 +35245,7 @@
       </c>
       <c r="Q267" s="2"/>
       <c r="R267" t="s" s="2">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="S267" t="s" s="2">
         <v>79</v>
@@ -35318,10 +35322,10 @@
     </row>
     <row r="268" hidden="true">
       <c r="A268" t="s" s="2">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B268" t="s" s="2">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" t="s" s="2">
@@ -35344,7 +35348,7 @@
         <v>79</v>
       </c>
       <c r="K268" t="s" s="2">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="L268" t="s" s="2">
         <v>235</v>
@@ -35436,10 +35440,10 @@
     </row>
     <row r="269" hidden="true">
       <c r="A269" t="s" s="2">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B269" t="s" s="2">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" t="s" s="2">
@@ -35465,10 +35469,10 @@
         <v>180</v>
       </c>
       <c r="L269" t="s" s="2">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="M269" t="s" s="2">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="N269" s="2"/>
       <c r="O269" s="2"/>
@@ -35480,7 +35484,7 @@
         <v>79</v>
       </c>
       <c r="S269" t="s" s="2">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="T269" t="s" s="2">
         <v>79</v>
@@ -35498,10 +35502,10 @@
         <v>325</v>
       </c>
       <c r="Y269" t="s" s="2">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="Z269" t="s" s="2">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="AA269" t="s" s="2">
         <v>79</v>
@@ -35519,7 +35523,7 @@
         <v>79</v>
       </c>
       <c r="AF269" t="s" s="2">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="AG269" t="s" s="2">
         <v>80</v>
@@ -35528,7 +35532,7 @@
         <v>91</v>
       </c>
       <c r="AI269" t="s" s="2">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="AJ269" t="s" s="2">
         <v>103</v>
@@ -35540,13 +35544,13 @@
         <v>79</v>
       </c>
       <c r="AM269" t="s" s="2">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="AN269" t="s" s="2">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="AO269" t="s" s="2">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="AP269" t="s" s="2">
         <v>79</v>
@@ -35554,10 +35558,10 @@
     </row>
     <row r="270" hidden="true">
       <c r="A270" t="s" s="2">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B270" t="s" s="2">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" t="s" s="2">
@@ -35583,16 +35587,16 @@
         <v>105</v>
       </c>
       <c r="L270" t="s" s="2">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="M270" t="s" s="2">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="N270" t="s" s="2">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="O270" t="s" s="2">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="P270" t="s" s="2">
         <v>79</v>
@@ -35641,7 +35645,7 @@
         <v>79</v>
       </c>
       <c r="AF270" t="s" s="2">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="AG270" t="s" s="2">
         <v>80</v>
@@ -35662,10 +35666,10 @@
         <v>79</v>
       </c>
       <c r="AM270" t="s" s="2">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="AN270" t="s" s="2">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="AO270" t="s" s="2">
         <v>358</v>
@@ -35676,10 +35680,10 @@
     </row>
     <row r="271" hidden="true">
       <c r="A271" t="s" s="2">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B271" t="s" s="2">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" t="s" s="2">
@@ -35705,16 +35709,16 @@
         <v>180</v>
       </c>
       <c r="L271" t="s" s="2">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="M271" t="s" s="2">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="N271" t="s" s="2">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="O271" t="s" s="2">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="P271" t="s" s="2">
         <v>79</v>
@@ -35742,10 +35746,10 @@
         <v>325</v>
       </c>
       <c r="Y271" t="s" s="2">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="Z271" t="s" s="2">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="AA271" t="s" s="2">
         <v>79</v>
@@ -35763,7 +35767,7 @@
         <v>79</v>
       </c>
       <c r="AF271" t="s" s="2">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="AG271" t="s" s="2">
         <v>80</v>
@@ -35784,13 +35788,13 @@
         <v>79</v>
       </c>
       <c r="AM271" t="s" s="2">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="AN271" t="s" s="2">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="AO271" t="s" s="2">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="AP271" t="s" s="2">
         <v>79</v>
@@ -35798,10 +35802,10 @@
     </row>
     <row r="272" hidden="true">
       <c r="A272" t="s" s="2">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B272" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" t="s" s="2">
@@ -35824,16 +35828,16 @@
         <v>92</v>
       </c>
       <c r="K272" t="s" s="2">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="L272" t="s" s="2">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="M272" t="s" s="2">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="N272" t="s" s="2">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="O272" s="2"/>
       <c r="P272" t="s" s="2">
@@ -35883,7 +35887,7 @@
         <v>79</v>
       </c>
       <c r="AF272" t="s" s="2">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="AG272" t="s" s="2">
         <v>80</v>
@@ -35918,10 +35922,10 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B273" t="s" s="2">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" t="s" s="2">
@@ -35947,10 +35951,10 @@
         <v>234</v>
       </c>
       <c r="L273" t="s" s="2">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="M273" t="s" s="2">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="N273" s="2"/>
       <c r="O273" s="2"/>
@@ -36001,7 +36005,7 @@
         <v>79</v>
       </c>
       <c r="AF273" t="s" s="2">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AG273" t="s" s="2">
         <v>80</v>
@@ -36025,7 +36029,7 @@
         <v>203</v>
       </c>
       <c r="AN273" t="s" s="2">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AO273" t="s" s="2">
         <v>365</v>
@@ -36036,10 +36040,10 @@
     </row>
     <row r="274" hidden="true">
       <c r="A274" t="s" s="2">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B274" t="s" s="2">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" t="s" s="2">
@@ -36062,19 +36066,19 @@
         <v>79</v>
       </c>
       <c r="K274" t="s" s="2">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="L274" t="s" s="2">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="M274" t="s" s="2">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="N274" t="s" s="2">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="O274" t="s" s="2">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="P274" t="s" s="2">
         <v>79</v>
@@ -36123,7 +36127,7 @@
         <v>79</v>
       </c>
       <c r="AF274" t="s" s="2">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="AG274" t="s" s="2">
         <v>80</v>
@@ -36135,22 +36139,22 @@
         <v>212</v>
       </c>
       <c r="AJ274" t="s" s="2">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="AK274" t="s" s="2">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="AL274" t="s" s="2">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="AM274" t="s" s="2">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="AN274" t="s" s="2">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="AO274" t="s" s="2">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="AP274" t="s" s="2">
         <v>79</v>
@@ -36158,10 +36162,10 @@
     </row>
     <row r="275" hidden="true">
       <c r="A275" t="s" s="2">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B275" t="s" s="2">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" t="s" s="2">
@@ -36184,17 +36188,17 @@
         <v>92</v>
       </c>
       <c r="K275" t="s" s="2">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="L275" t="s" s="2">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="M275" t="s" s="2">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="N275" s="2"/>
       <c r="O275" t="s" s="2">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="P275" t="s" s="2">
         <v>79</v>
@@ -36243,7 +36247,7 @@
         <v>79</v>
       </c>
       <c r="AF275" t="s" s="2">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="AG275" t="s" s="2">
         <v>80</v>
@@ -36267,7 +36271,7 @@
         <v>547</v>
       </c>
       <c r="AN275" t="s" s="2">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="AO275" t="s" s="2">
         <v>109</v>
@@ -36278,10 +36282,10 @@
     </row>
     <row r="276" hidden="true">
       <c r="A276" t="s" s="2">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B276" t="s" s="2">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" t="s" s="2">
@@ -36396,10 +36400,10 @@
     </row>
     <row r="277" hidden="true">
       <c r="A277" t="s" s="2">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B277" t="s" s="2">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" t="s" s="2">
@@ -36516,10 +36520,10 @@
     </row>
     <row r="278" hidden="true">
       <c r="A278" t="s" s="2">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B278" t="s" s="2">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" t="s" s="2">
@@ -36545,13 +36549,13 @@
         <v>105</v>
       </c>
       <c r="L278" t="s" s="2">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="M278" t="s" s="2">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="N278" t="s" s="2">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="O278" s="2"/>
       <c r="P278" t="s" s="2">
@@ -36601,7 +36605,7 @@
         <v>79</v>
       </c>
       <c r="AF278" t="s" s="2">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="AG278" t="s" s="2">
         <v>80</v>
@@ -36610,7 +36614,7 @@
         <v>91</v>
       </c>
       <c r="AI278" t="s" s="2">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="AJ278" t="s" s="2">
         <v>103</v>
@@ -36636,10 +36640,10 @@
     </row>
     <row r="279" hidden="true">
       <c r="A279" t="s" s="2">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B279" t="s" s="2">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" t="s" s="2">
@@ -36665,13 +36669,13 @@
         <v>138</v>
       </c>
       <c r="L279" t="s" s="2">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="M279" t="s" s="2">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="N279" t="s" s="2">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="O279" s="2"/>
       <c r="P279" t="s" s="2">
@@ -36719,7 +36723,7 @@
         <v>79</v>
       </c>
       <c r="AF279" t="s" s="2">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="AG279" t="s" s="2">
         <v>80</v>
@@ -36754,10 +36758,10 @@
     </row>
     <row r="280" hidden="true">
       <c r="A280" t="s" s="2">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B280" t="s" s="2">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" t="s" s="2">
@@ -36783,13 +36787,13 @@
         <v>307</v>
       </c>
       <c r="L280" t="s" s="2">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="M280" t="s" s="2">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="N280" t="s" s="2">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O280" s="2"/>
       <c r="P280" t="s" s="2">
@@ -36839,7 +36843,7 @@
         <v>79</v>
       </c>
       <c r="AF280" t="s" s="2">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="AG280" t="s" s="2">
         <v>80</v>
@@ -36863,7 +36867,7 @@
         <v>79</v>
       </c>
       <c r="AN280" t="s" s="2">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="AO280" t="s" s="2">
         <v>79</v>
@@ -36874,10 +36878,10 @@
     </row>
     <row r="281" hidden="true">
       <c r="A281" t="s" s="2">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B281" t="s" s="2">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" t="s" s="2">
@@ -36903,13 +36907,13 @@
         <v>105</v>
       </c>
       <c r="L281" t="s" s="2">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="M281" t="s" s="2">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="N281" t="s" s="2">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="O281" s="2"/>
       <c r="P281" t="s" s="2">
@@ -36959,7 +36963,7 @@
         <v>79</v>
       </c>
       <c r="AF281" t="s" s="2">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="AG281" t="s" s="2">
         <v>80</v>
@@ -36994,10 +36998,10 @@
     </row>
     <row r="282" hidden="true">
       <c r="A282" t="s" s="2">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B282" t="s" s="2">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" t="s" s="2">
@@ -37020,19 +37024,19 @@
         <v>79</v>
       </c>
       <c r="K282" t="s" s="2">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="L282" t="s" s="2">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="M282" t="s" s="2">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="N282" t="s" s="2">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="O282" t="s" s="2">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="P282" t="s" s="2">
         <v>79</v>
@@ -37081,7 +37085,7 @@
         <v>79</v>
       </c>
       <c r="AF282" t="s" s="2">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="AG282" t="s" s="2">
         <v>80</v>
@@ -37105,7 +37109,7 @@
         <v>79</v>
       </c>
       <c r="AN282" t="s" s="2">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="AO282" t="s" s="2">
         <v>79</v>
@@ -37116,10 +37120,10 @@
     </row>
     <row r="283" hidden="true">
       <c r="A283" t="s" s="2">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B283" t="s" s="2">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" t="s" s="2">
@@ -37234,10 +37238,10 @@
     </row>
     <row r="284" hidden="true">
       <c r="A284" t="s" s="2">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B284" t="s" s="2">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" t="s" s="2">
@@ -37354,14 +37358,14 @@
     </row>
     <row r="285" hidden="true">
       <c r="A285" t="s" s="2">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B285" t="s" s="2">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" t="s" s="2">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E285" s="2"/>
       <c r="F285" t="s" s="2">
@@ -37383,10 +37387,10 @@
         <v>112</v>
       </c>
       <c r="L285" t="s" s="2">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="M285" t="s" s="2">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="N285" t="s" s="2">
         <v>115</v>
@@ -37441,7 +37445,7 @@
         <v>79</v>
       </c>
       <c r="AF285" t="s" s="2">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="AG285" t="s" s="2">
         <v>80</v>
@@ -37476,10 +37480,10 @@
     </row>
     <row r="286" hidden="true">
       <c r="A286" t="s" s="2">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B286" t="s" s="2">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" t="s" s="2">
@@ -37505,14 +37509,14 @@
         <v>331</v>
       </c>
       <c r="L286" t="s" s="2">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="M286" t="s" s="2">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="N286" s="2"/>
       <c r="O286" t="s" s="2">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="P286" t="s" s="2">
         <v>79</v>
@@ -37540,10 +37544,10 @@
         <v>162</v>
       </c>
       <c r="Y286" t="s" s="2">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="Z286" t="s" s="2">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="AA286" t="s" s="2">
         <v>79</v>
@@ -37561,7 +37565,7 @@
         <v>79</v>
       </c>
       <c r="AF286" t="s" s="2">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="AG286" t="s" s="2">
         <v>80</v>
@@ -37585,7 +37589,7 @@
         <v>79</v>
       </c>
       <c r="AN286" t="s" s="2">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="AO286" t="s" s="2">
         <v>79</v>
@@ -37596,10 +37600,10 @@
     </row>
     <row r="287" hidden="true">
       <c r="A287" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B287" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" t="s" s="2">
@@ -37622,17 +37626,17 @@
         <v>79</v>
       </c>
       <c r="K287" t="s" s="2">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="L287" t="s" s="2">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="M287" t="s" s="2">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="N287" s="2"/>
       <c r="O287" t="s" s="2">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="P287" t="s" s="2">
         <v>79</v>
@@ -37681,7 +37685,7 @@
         <v>79</v>
       </c>
       <c r="AF287" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="AG287" t="s" s="2">
         <v>80</v>
@@ -37702,10 +37706,10 @@
         <v>79</v>
       </c>
       <c r="AM287" t="s" s="2">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="AN287" t="s" s="2">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="AO287" t="s" s="2">
         <v>79</v>
@@ -37716,10 +37720,10 @@
     </row>
     <row r="288" hidden="true">
       <c r="A288" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B288" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" t="s" s="2">
@@ -37745,14 +37749,14 @@
         <v>713</v>
       </c>
       <c r="L288" t="s" s="2">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="M288" t="s" s="2">
         <v>715</v>
       </c>
       <c r="N288" s="2"/>
       <c r="O288" t="s" s="2">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="P288" t="s" s="2">
         <v>79</v>
@@ -37801,7 +37805,7 @@
         <v>79</v>
       </c>
       <c r="AF288" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="AG288" t="s" s="2">
         <v>80</v>
@@ -37813,7 +37817,7 @@
         <v>212</v>
       </c>
       <c r="AJ288" t="s" s="2">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="AK288" t="s" s="2">
         <v>79</v>
@@ -37822,13 +37826,13 @@
         <v>79</v>
       </c>
       <c r="AM288" t="s" s="2">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="AN288" t="s" s="2">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="AO288" t="s" s="2">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="AP288" t="s" s="2">
         <v>79</v>
@@ -37836,10 +37840,10 @@
     </row>
     <row r="289" hidden="true">
       <c r="A289" t="s" s="2">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B289" t="s" s="2">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" t="s" s="2">
@@ -37862,19 +37866,19 @@
         <v>79</v>
       </c>
       <c r="K289" t="s" s="2">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L289" t="s" s="2">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="M289" t="s" s="2">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="N289" t="s" s="2">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="O289" t="s" s="2">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="P289" t="s" s="2">
         <v>79</v>
@@ -37923,7 +37927,7 @@
         <v>79</v>
       </c>
       <c r="AF289" t="s" s="2">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="AG289" t="s" s="2">
         <v>80</v>
@@ -37944,13 +37948,13 @@
         <v>79</v>
       </c>
       <c r="AM289" t="s" s="2">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="AN289" t="s" s="2">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="AO289" t="s" s="2">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="AP289" t="s" s="2">
         <v>79</v>
@@ -37958,10 +37962,10 @@
     </row>
     <row r="290" hidden="true">
       <c r="A290" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B290" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" t="s" s="2">
@@ -37984,17 +37988,17 @@
         <v>79</v>
       </c>
       <c r="K290" t="s" s="2">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="L290" t="s" s="2">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="M290" t="s" s="2">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="N290" s="2"/>
       <c r="O290" t="s" s="2">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="P290" t="s" s="2">
         <v>79</v>
@@ -38043,7 +38047,7 @@
         <v>79</v>
       </c>
       <c r="AF290" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="AG290" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
test new telecom error 95f8b8b11b591b4f5338120c97dac2b60a453955
</commit_message>
<xml_diff>
--- a/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-organization.xlsx
+++ b/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-organization.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-12T09:26:25+00:00</t>
+    <t>2024-10-29T10:53:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2248,7 +2248,7 @@
   </si>
   <si>
     <t>pattern:system}
-pattern:extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-contact-point-email-type').value}</t>
+exists:extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-contact-point-email-type')}</t>
   </si>
   <si>
     <t>cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}
@@ -3304,7 +3304,7 @@
     <col min="25" max="25" width="98.61328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="108.3828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="96.68359375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="89.67578125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>